<commit_message>
add data driven input example and fix bug in pipe delimited file parsing
</commit_message>
<xml_diff>
--- a/data/example.xlsx
+++ b/data/example.xlsx
@@ -408,11 +408,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:D3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="13.83203125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="2" spans="1:4">
       <c r="A2" t="s">

</xml_diff>